<commit_message>
Atualizando dados com jogos de 07/04/2019
</commit_message>
<xml_diff>
--- a/CBLOL_BRASIL_2019.xlsx
+++ b/CBLOL_BRASIL_2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BF7259-3573-40F2-A97F-95B6A5F36D45}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9992C50E-F69C-4C0E-B659-D5DFC1EF4615}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="11520" windowHeight="10188" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Games" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="140">
   <si>
     <t xml:space="preserve">       Semana 1</t>
   </si>
@@ -1033,7 +1033,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1186,7 +1186,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1479,10 +1478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C88"/>
+  <dimension ref="A1:C93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2423,35 +2422,90 @@
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" s="83" t="s">
+      <c r="A86" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B86" s="84" t="s">
+      <c r="B86" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="C86" s="82">
+      <c r="C86" s="72">
         <v>-1</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" s="83" t="s">
+      <c r="A87" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B87" s="84" t="s">
+      <c r="B87" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="C87" s="82">
+      <c r="C87" s="72">
         <v>-1</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" s="83" t="s">
+      <c r="A88" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B88" s="84" t="s">
+      <c r="B88" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="C88" s="82">
+      <c r="C88" s="72">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="82" t="s">
+        <v>15</v>
+      </c>
+      <c r="B89" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="C89" s="72">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="82" t="s">
+        <v>15</v>
+      </c>
+      <c r="B90" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="C90" s="72">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="82" t="s">
+        <v>15</v>
+      </c>
+      <c r="B91" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="C91" s="72">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="B92" s="83" t="s">
+        <v>15</v>
+      </c>
+      <c r="C92" s="72">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="B93" s="83" t="s">
+        <v>15</v>
+      </c>
+      <c r="C93" s="72">
         <v>-1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tudo atualizado ate 14/04/2019
</commit_message>
<xml_diff>
--- a/CBLOL_BRASIL_2019.xlsx
+++ b/CBLOL_BRASIL_2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9992C50E-F69C-4C0E-B659-D5DFC1EF4615}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE434373-0099-4C00-9023-F5FD3BD45B63}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Games" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="140">
   <si>
     <t xml:space="preserve">       Semana 1</t>
   </si>
@@ -1033,7 +1033,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1190,6 +1190,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1478,10 +1487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="F93" sqref="F93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2422,13 +2431,13 @@
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" s="76" t="s">
-        <v>18</v>
-      </c>
-      <c r="B86" s="50" t="s">
+      <c r="A86" s="74" t="s">
+        <v>18</v>
+      </c>
+      <c r="B86" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="C86" s="72">
+      <c r="C86" s="71">
         <v>-1</v>
       </c>
     </row>
@@ -2436,7 +2445,7 @@
       <c r="A87" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B87" s="50" t="s">
+      <c r="B87" s="84" t="s">
         <v>20</v>
       </c>
       <c r="C87" s="72">
@@ -2447,7 +2456,7 @@
       <c r="A88" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B88" s="50" t="s">
+      <c r="B88" s="84" t="s">
         <v>20</v>
       </c>
       <c r="C88" s="72">
@@ -2458,7 +2467,7 @@
       <c r="A89" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="B89" s="50" t="s">
+      <c r="B89" s="84" t="s">
         <v>117</v>
       </c>
       <c r="C89" s="72">
@@ -2469,7 +2478,7 @@
       <c r="A90" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="B90" s="50" t="s">
+      <c r="B90" s="84" t="s">
         <v>117</v>
       </c>
       <c r="C90" s="72">
@@ -2506,6 +2515,61 @@
         <v>15</v>
       </c>
       <c r="C93" s="72">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="82" t="s">
+        <v>15</v>
+      </c>
+      <c r="B94" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="C94" s="72">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="82" t="s">
+        <v>15</v>
+      </c>
+      <c r="B95" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="C95" s="72">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="82" t="s">
+        <v>15</v>
+      </c>
+      <c r="B96" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="C96" s="72">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="82" t="s">
+        <v>18</v>
+      </c>
+      <c r="B97" s="83" t="s">
+        <v>15</v>
+      </c>
+      <c r="C97" s="72">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="B98" s="86" t="s">
+        <v>15</v>
+      </c>
+      <c r="C98" s="73">
         <v>-1</v>
       </c>
     </row>

</xml_diff>